<commit_message>
Separate inventory items per project - each project now has its own Master_Items file
</commit_message>
<xml_diff>
--- a/projects/cocacola_Transactions.xlsx
+++ b/projects/cocacola_Transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5390,6 +5390,45 @@
       </c>
       <c r="K101" t="inlineStr"/>
     </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>1765134295</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>cocacola</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2025-12-07 21:04:55</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>بويات</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>تشطيبات</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>دخول</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>9</v>
+      </c>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="n">
+        <v>365</v>
+      </c>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>